<commit_message>
modified non reporting municipalities translations
</commit_message>
<xml_diff>
--- a/src/Data/country_data.xlsx
+++ b/src/Data/country_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment/src/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\OneDrive\Documents\mr-risk-assessment\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{ECB9B45C-EA6E-2B4F-B642-69CC5184D9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CDAE545-0498-478B-BFA1-6E1FC662BDE4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB21942-1E30-4A3E-86F4-D1438ED0EF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -3136,8 +3136,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScale="139" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3403,7 +3403,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -9138,21 +9138,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007C69FE739999C447A76F1EF8B3FD66E4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cbd048430c8551c34c2c3c8571f1b260">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4655c133-e14e-4d88-8fbc-c3b347145ec5" xmlns:ns4="64ced670-a384-4657-ba0f-fc07d30f5a44" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5457dbb80d17598a17de4d439e456cf2" ns3:_="" ns4:_="">
     <xsd:import namespace="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
@@ -9375,10 +9360,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C9E008-75C3-4280-8CCC-7498B59407BC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
+    <ds:schemaRef ds:uri="64ced670-a384-4657-ba0f-fc07d30f5a44"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9401,20 +9412,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1C9E008-75C3-4280-8CCC-7498B59407BC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6264E33-6917-4678-8EC8-8D88A2F9795C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4655c133-e14e-4d88-8fbc-c3b347145ec5"/>
-    <ds:schemaRef ds:uri="64ced670-a384-4657-ba0f-fc07d30f5a44"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>